<commit_message>
daily entry + data
</commit_message>
<xml_diff>
--- a/Raw_SRB_data/O2_selumetinib/Selumetinib_SRB_data.xlsx
+++ b/Raw_SRB_data/O2_selumetinib/Selumetinib_SRB_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7650" windowHeight="3720" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="S1" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,11 @@
     <sheet name="S7" sheetId="7" r:id="rId7"/>
     <sheet name="S8" sheetId="8" r:id="rId8"/>
     <sheet name="S9" sheetId="9" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
+    <sheet name="S10" sheetId="12" r:id="rId10"/>
+    <sheet name="S11" sheetId="13" r:id="rId11"/>
+    <sheet name="S12" sheetId="14" r:id="rId12"/>
+    <sheet name="S13" sheetId="15" r:id="rId13"/>
+    <sheet name="Troubleshooting" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Crizotinib</t>
   </si>
@@ -116,26 +120,47 @@
     <t>Day  1 date: 12/8/19</t>
   </si>
   <si>
-    <t>Selumetinib 10 P9</t>
-  </si>
-  <si>
-    <t>Selumetinib 11 P9</t>
-  </si>
-  <si>
-    <t>Selumetinib 12 P10</t>
-  </si>
-  <si>
     <t>shaken too much</t>
   </si>
   <si>
-    <t>Selumetinib 13 P12</t>
+    <t>Selumetinib - troubleshooting</t>
+  </si>
+  <si>
+    <t>Day  1 date: 16/12/19</t>
+  </si>
+  <si>
+    <t>Passage #13</t>
+  </si>
+  <si>
+    <t>Replicate # 10</t>
+  </si>
+  <si>
+    <t>Day  1 date: 21/11/19</t>
+  </si>
+  <si>
+    <t>Replicate # 11</t>
+  </si>
+  <si>
+    <t>Day  1 date: 25/11/19</t>
+  </si>
+  <si>
+    <t>Replicate # 12</t>
+  </si>
+  <si>
+    <t>Day  1 date: 28/11/19</t>
+  </si>
+  <si>
+    <t>Replicate # 13</t>
+  </si>
+  <si>
+    <t>Day  1 date: 2/12/19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +177,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -195,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -203,11 +236,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -218,6 +266,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,1567 +1165,2270 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33:W33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9:W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.8E-2</v>
+      </c>
+      <c r="B8">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.115</v>
+      </c>
+      <c r="E8">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="H8">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="I8">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="J8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="L8">
+        <v>5.5E-2</v>
+      </c>
+      <c r="N8">
+        <f>AVERAGE(B9:B13)</f>
+        <v>1.6015999999999999</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:W8" si="0">AVERAGE(C9:C13)</f>
+        <v>1.3498000000000001</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>1.2582</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>0.90939999999999999</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>0.78180000000000005</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>0.60140000000000005</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>0.47020000000000001</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>0.3654</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>0.26239999999999997</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="0"/>
+        <v>0.25179999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.06</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.4239999999999999</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.258</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.376</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.249</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="L9">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="N9" s="7">
+        <v>100</v>
+      </c>
+      <c r="O9" s="7">
+        <f>O8/1.6016*100</f>
+        <v>84.278221778221791</v>
+      </c>
+      <c r="P9" s="7">
+        <f t="shared" ref="P9:W9" si="1">P8/1.6016*100</f>
+        <v>78.558941058941073</v>
+      </c>
+      <c r="Q9" s="7">
+        <f t="shared" si="1"/>
+        <v>56.780719280719282</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" si="1"/>
+        <v>48.813686313686318</v>
+      </c>
+      <c r="S9" s="7">
+        <f t="shared" si="1"/>
+        <v>37.549950049950056</v>
+      </c>
+      <c r="T9" s="7">
+        <f t="shared" si="1"/>
+        <v>29.358141858141863</v>
+      </c>
+      <c r="U9" s="7">
+        <f t="shared" si="1"/>
+        <v>22.814685314685317</v>
+      </c>
+      <c r="V9" s="7">
+        <f t="shared" si="1"/>
+        <v>16.383616383616381</v>
+      </c>
+      <c r="W9" s="7">
+        <f t="shared" si="1"/>
+        <v>15.721778221778221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6.3E-2</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.597</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.331</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.88600000000000001</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.23899999999999999</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.23</v>
+      </c>
+      <c r="L10">
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.5549999999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.367</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.2709999999999999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.36499999999999999</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="L11">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1.629</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1.3360000000000001</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.623</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="L12">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1.587</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.2909999999999999</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1.22</v>
+      </c>
+      <c r="E13" s="6">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0.255</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="L13">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="B14">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C14">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="D14">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="E14">
+        <v>6.2E-2</v>
+      </c>
+      <c r="F14">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="G14">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="H14">
+        <v>9.4E-2</v>
+      </c>
+      <c r="I14">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="J14">
+        <v>7.8E-2</v>
+      </c>
+      <c r="K14">
+        <v>7.8E-2</v>
+      </c>
+      <c r="L14">
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="B15">
+        <v>0.05</v>
+      </c>
+      <c r="C15">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="G15">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="H15">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I15">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="J15">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="K15">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="L15">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="B8">
+        <v>0.106</v>
+      </c>
+      <c r="C8">
+        <v>0.125</v>
+      </c>
+      <c r="D8">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.17</v>
+      </c>
+      <c r="F8">
+        <v>0.186</v>
+      </c>
+      <c r="G8">
+        <v>0.22800000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.182</v>
+      </c>
+      <c r="I8">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="J8">
+        <v>0.121</v>
+      </c>
+      <c r="K8">
+        <v>0.115</v>
+      </c>
+      <c r="L8">
+        <v>0.111</v>
+      </c>
+      <c r="N8">
+        <f>AVERAGE(B9:B11)</f>
+        <v>1.5609999999999999</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:W8" si="0">AVERAGE(C9:C11)</f>
+        <v>1.27</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>1.1536666666666664</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>1.042</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>1.1143333333333334</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>0.58966666666666667</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>0.46</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="0"/>
+        <v>0.39833333333333337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.107</v>
+      </c>
+      <c r="B9">
+        <v>1.591</v>
+      </c>
+      <c r="C9">
+        <v>1.194</v>
+      </c>
+      <c r="D9">
+        <v>1.5189999999999999</v>
+      </c>
+      <c r="E9">
+        <v>1.0409999999999999</v>
+      </c>
+      <c r="F9">
+        <v>1.089</v>
+      </c>
+      <c r="G9">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="H9">
+        <v>0.78</v>
+      </c>
+      <c r="I9">
+        <v>0.6</v>
+      </c>
+      <c r="J9">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="K9">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="L9">
+        <v>0.1</v>
+      </c>
+      <c r="N9">
+        <v>100</v>
+      </c>
+      <c r="O9">
+        <f>O8/1.561*100</f>
+        <v>81.358103779628436</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:W9" si="1">P8/1.561*100</f>
+        <v>73.905616058082416</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>66.752081998718765</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>71.385863762545384</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>59.192825112107627</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>48.814862267777073</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="1"/>
+        <v>37.774930600042708</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="1"/>
+        <v>29.468289557975659</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="1"/>
+        <v>25.517830450565882</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.122</v>
+      </c>
+      <c r="B10">
+        <v>1.4910000000000001</v>
+      </c>
+      <c r="C10">
+        <v>1.298</v>
+      </c>
+      <c r="D10">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="E10">
+        <v>1.0469999999999999</v>
+      </c>
+      <c r="F10">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G10">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H10">
+        <v>0.752</v>
+      </c>
+      <c r="I10">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="J10">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="K10">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="L10">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="N10" s="11" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.155</v>
+      </c>
+      <c r="B11">
+        <v>1.601</v>
+      </c>
+      <c r="C11">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="D11">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="E11">
+        <v>1.038</v>
+      </c>
+      <c r="F11">
+        <v>1.1339999999999999</v>
+      </c>
+      <c r="G11">
+        <v>0.92100000000000004</v>
+      </c>
+      <c r="H11">
+        <v>0.754</v>
+      </c>
+      <c r="I11">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="J11">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="K11">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="L11">
+        <v>0.14899999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="B12">
+        <v>0.151</v>
+      </c>
+      <c r="C12">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="D12">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.19</v>
+      </c>
+      <c r="F12">
+        <v>0.186</v>
+      </c>
+      <c r="G12">
+        <v>0.16</v>
+      </c>
+      <c r="H12">
+        <v>0.185</v>
+      </c>
+      <c r="I12">
+        <v>0.217</v>
+      </c>
+      <c r="J12">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="K12">
+        <v>0.245</v>
+      </c>
+      <c r="L12">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="B13">
+        <v>0.153</v>
+      </c>
+      <c r="C13">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="D13">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.183</v>
+      </c>
+      <c r="F13">
+        <v>0.19</v>
+      </c>
+      <c r="G13">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="H13">
+        <v>0.20699999999999999</v>
+      </c>
+      <c r="I13">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="J13">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="K13">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="L13">
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.124</v>
+      </c>
+      <c r="B14">
+        <v>0.157</v>
+      </c>
+      <c r="C14">
+        <v>0.153</v>
+      </c>
+      <c r="D14">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="E14">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F14">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.128</v>
+      </c>
+      <c r="H14">
+        <v>0.161</v>
+      </c>
+      <c r="I14">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="J14">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="K14">
+        <v>0.155</v>
+      </c>
+      <c r="L14">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.112</v>
+      </c>
+      <c r="B15">
+        <v>0.124</v>
+      </c>
+      <c r="C15">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D15">
+        <v>0.15</v>
+      </c>
+      <c r="E15">
+        <v>0.151</v>
+      </c>
+      <c r="F15">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.155</v>
+      </c>
+      <c r="H15">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="I15">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="J15">
+        <v>0.155</v>
+      </c>
+      <c r="K15">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="L15">
+        <v>0.11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>7.8E-2</v>
-      </c>
-      <c r="B2">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="C2">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <v>0.111</v>
+      </c>
+      <c r="D8">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.1</v>
+      </c>
+      <c r="F8">
+        <v>0.104</v>
+      </c>
+      <c r="G8">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="H8">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="I8">
+        <v>9.4E-2</v>
+      </c>
+      <c r="J8">
+        <v>0.107</v>
+      </c>
+      <c r="K8">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="L8">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="N8">
+        <f>AVERAGE(B9:B11)</f>
+        <v>1.8873333333333333</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ref="O8:W8" si="0">AVERAGE(C9:C11)</f>
+        <v>1.6706666666666667</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>1.5486666666666666</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>1.0773333333333333</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>0.95866666666666678</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>0.73133333333333328</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>0.60133333333333339</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>0.49933333333333341</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>0.37833333333333335</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="0"/>
+        <v>0.33300000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9.4E-2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.9930000000000001</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.667</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.51</v>
+      </c>
+      <c r="E9" s="6">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.193</v>
+      </c>
+      <c r="N9" s="7">
+        <v>100</v>
+      </c>
+      <c r="O9" s="7">
+        <f>O8/1.887333*100</f>
+        <v>88.519973246198035</v>
+      </c>
+      <c r="P9" s="7">
+        <f t="shared" ref="P9:W9" si="1">P8/1.887333*100</f>
+        <v>82.055825159983257</v>
+      </c>
+      <c r="Q9" s="7">
+        <f t="shared" si="1"/>
+        <v>57.082313154770958</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" si="1"/>
+        <v>50.794781136485547</v>
+      </c>
+      <c r="S9" s="7">
+        <f t="shared" si="1"/>
+        <v>38.749565303702809</v>
+      </c>
+      <c r="T9" s="7">
+        <f t="shared" si="1"/>
+        <v>31.861538654457554</v>
+      </c>
+      <c r="U9" s="7">
+        <f t="shared" si="1"/>
+        <v>26.457086975818971</v>
+      </c>
+      <c r="V9" s="7">
+        <f t="shared" si="1"/>
+        <v>20.045923709982997</v>
+      </c>
+      <c r="W9" s="7">
+        <f t="shared" si="1"/>
+        <v>17.643945186143622</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.127</v>
+      </c>
+      <c r="B10" s="6">
+        <v>1.804</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.675</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.58</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="L10">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.107</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.865</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.67</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.556</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1.0649999999999999</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.37</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="L11">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.08</v>
+      </c>
+      <c r="B12">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0.122</v>
+      </c>
+      <c r="E12">
+        <v>0.192</v>
+      </c>
+      <c r="F12">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.114</v>
+      </c>
+      <c r="H12">
+        <v>0.123</v>
+      </c>
+      <c r="I12">
+        <v>0.121</v>
+      </c>
+      <c r="J12">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="K12">
+        <v>0.159</v>
+      </c>
+      <c r="L12">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.105</v>
+      </c>
+      <c r="B13">
+        <v>0.108</v>
+      </c>
+      <c r="C13">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F13">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G13">
+        <v>0.159</v>
+      </c>
+      <c r="H13">
+        <v>0.158</v>
+      </c>
+      <c r="I13">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="J13">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="K13">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="L13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.108</v>
+      </c>
+      <c r="B14">
+        <v>0.123</v>
+      </c>
+      <c r="C14">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.159</v>
+      </c>
+      <c r="E14">
         <v>0.11600000000000001</v>
       </c>
-      <c r="D2">
-        <v>0.115</v>
-      </c>
-      <c r="E2">
+      <c r="F14">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.13</v>
+      </c>
+      <c r="H14">
+        <v>0.124</v>
+      </c>
+      <c r="I14">
+        <v>0.13</v>
+      </c>
+      <c r="J14">
         <v>0.13200000000000001</v>
       </c>
-      <c r="F2">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="G2">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="H2">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="I2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="J2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K2">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="L2">
-        <v>5.5E-2</v>
-      </c>
-      <c r="N2">
-        <f>AVERAGE(B3:B7)</f>
-        <v>1.6015999999999999</v>
-      </c>
-      <c r="O2">
-        <f t="shared" ref="O2:W2" si="0">AVERAGE(C3:C7)</f>
-        <v>1.3498000000000001</v>
-      </c>
-      <c r="P2">
-        <f t="shared" si="0"/>
-        <v>1.2582</v>
-      </c>
-      <c r="Q2">
-        <f t="shared" si="0"/>
-        <v>0.90939999999999999</v>
-      </c>
-      <c r="R2">
-        <f t="shared" si="0"/>
-        <v>0.78180000000000005</v>
-      </c>
-      <c r="S2">
-        <f t="shared" si="0"/>
-        <v>0.60140000000000005</v>
-      </c>
-      <c r="T2">
-        <f t="shared" si="0"/>
-        <v>0.47020000000000001</v>
-      </c>
-      <c r="U2">
-        <f t="shared" si="0"/>
-        <v>0.3654</v>
-      </c>
-      <c r="V2">
-        <f t="shared" si="0"/>
-        <v>0.26239999999999997</v>
-      </c>
-      <c r="W2">
-        <f t="shared" si="0"/>
-        <v>0.25179999999999997</v>
-      </c>
+      <c r="K14">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="L14">
+        <v>0.111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.112</v>
+      </c>
+      <c r="B15">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.157</v>
+      </c>
+      <c r="D15">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="E15">
+        <v>0.113</v>
+      </c>
+      <c r="F15">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="H15">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="I15">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="J15">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="K15">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L15">
+        <v>0.112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.06</v>
-      </c>
-      <c r="B3">
-        <v>1.64</v>
-      </c>
-      <c r="C3">
-        <v>1.4239999999999999</v>
-      </c>
-      <c r="D3">
-        <v>1.258</v>
-      </c>
-      <c r="E3">
-        <v>0.94199999999999995</v>
-      </c>
-      <c r="F3">
-        <v>0.77100000000000002</v>
-      </c>
-      <c r="G3">
-        <v>0.59399999999999997</v>
-      </c>
-      <c r="H3">
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="I3">
-        <v>0.376</v>
-      </c>
-      <c r="J3">
-        <v>0.249</v>
-      </c>
-      <c r="K3">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="L3">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="N3">
-        <v>100</v>
-      </c>
-      <c r="O3">
-        <f>O2/1.6016*100</f>
-        <v>84.278221778221791</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:W3" si="1">P2/1.6016*100</f>
-        <v>78.558941058941073</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" si="1"/>
-        <v>56.780719280719282</v>
-      </c>
-      <c r="R3">
-        <f t="shared" si="1"/>
-        <v>48.813686313686318</v>
-      </c>
-      <c r="S3">
-        <f t="shared" si="1"/>
-        <v>37.549950049950056</v>
-      </c>
-      <c r="T3">
-        <f t="shared" si="1"/>
-        <v>29.358141858141863</v>
-      </c>
-      <c r="U3">
-        <f t="shared" si="1"/>
-        <v>22.814685314685317</v>
-      </c>
-      <c r="V3">
-        <f t="shared" si="1"/>
-        <v>16.383616383616381</v>
-      </c>
-      <c r="W3">
-        <f t="shared" si="1"/>
-        <v>15.721778221778221</v>
-      </c>
+      <c r="A3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6.3E-2</v>
-      </c>
-      <c r="B4">
-        <v>1.597</v>
-      </c>
-      <c r="C4">
-        <v>1.331</v>
-      </c>
-      <c r="D4">
-        <v>1.3129999999999999</v>
-      </c>
-      <c r="E4">
-        <v>0.88600000000000001</v>
-      </c>
-      <c r="F4">
-        <v>0.79100000000000004</v>
-      </c>
-      <c r="G4">
-        <v>0.52400000000000002</v>
-      </c>
-      <c r="H4">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="I4">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="J4">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="K4">
-        <v>0.23</v>
-      </c>
-      <c r="L4">
-        <v>8.3000000000000004E-2</v>
-      </c>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="B5">
-        <v>1.5549999999999999</v>
-      </c>
-      <c r="C5">
-        <v>1.367</v>
-      </c>
-      <c r="D5">
-        <v>1.2709999999999999</v>
-      </c>
-      <c r="E5">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="F5">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="G5">
-        <v>0.69799999999999995</v>
-      </c>
-      <c r="H5">
-        <v>0.49</v>
-      </c>
-      <c r="I5">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="J5">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="K5">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="L5">
-        <v>5.0999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="B6">
-        <v>1.629</v>
-      </c>
-      <c r="C6">
-        <v>1.3360000000000001</v>
-      </c>
-      <c r="D6">
-        <v>1.2290000000000001</v>
-      </c>
-      <c r="E6">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="F6">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="G6">
-        <v>0.623</v>
-      </c>
-      <c r="H6">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="I6">
-        <v>0.36899999999999999</v>
-      </c>
-      <c r="J6">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="K6">
-        <v>0.25600000000000001</v>
-      </c>
-      <c r="L6">
-        <v>9.0999999999999998E-2</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7.1999999999999995E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="B7">
-        <v>1.587</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="C7">
-        <v>1.2909999999999999</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="D7">
-        <v>1.22</v>
+        <v>5.5E-2</v>
       </c>
       <c r="E7">
-        <v>0.89400000000000002</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="F7">
-        <v>0.78500000000000003</v>
+        <v>6.3E-2</v>
       </c>
       <c r="G7">
-        <v>0.56799999999999995</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="H7">
-        <v>0.45900000000000002</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="I7">
-        <v>0.36399999999999999</v>
+        <v>4.7E-2</v>
       </c>
       <c r="J7">
-        <v>0.255</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="K7">
-        <v>0.25900000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L7">
-        <v>5.6000000000000001E-2</v>
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="N7">
+        <f>AVERAGE(B8:B12)</f>
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ref="O7:W7" si="0">AVERAGE(C8:C12)</f>
+        <v>1.4758000000000002</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>1.3779999999999999</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>0.93599999999999994</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>0.82279999999999998</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>0.61080000000000001</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>0.5292</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>0.41259999999999997</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>0.31540000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="B8">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="C8">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="D8">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="E8">
-        <v>6.2E-2</v>
-      </c>
-      <c r="F8">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="G8">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="H8">
-        <v>9.4E-2</v>
-      </c>
-      <c r="I8">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="J8">
-        <v>7.8E-2</v>
-      </c>
-      <c r="K8">
-        <v>7.8E-2</v>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1.456</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.5069999999999999</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.355</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.32900000000000001</v>
       </c>
       <c r="L8">
-        <v>4.8000000000000001E-2</v>
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="N8" s="7">
+        <v>100</v>
+      </c>
+      <c r="O8" s="7">
+        <f>O7/1.525*100</f>
+        <v>96.773770491803305</v>
+      </c>
+      <c r="P8" s="7">
+        <f t="shared" ref="P8:W8" si="1">P7/1.525*100</f>
+        <v>90.360655737704917</v>
+      </c>
+      <c r="Q8" s="7">
+        <f t="shared" si="1"/>
+        <v>61.377049180327873</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="1"/>
+        <v>53.954098360655742</v>
+      </c>
+      <c r="S8" s="7">
+        <f t="shared" si="1"/>
+        <v>40.052459016393442</v>
+      </c>
+      <c r="T8" s="7">
+        <f t="shared" si="1"/>
+        <v>34.701639344262297</v>
+      </c>
+      <c r="U8" s="7">
+        <f t="shared" si="1"/>
+        <v>27.05573770491803</v>
+      </c>
+      <c r="V8" s="7">
+        <f t="shared" si="1"/>
+        <v>24.131147540983608</v>
+      </c>
+      <c r="W8" s="7">
+        <f t="shared" si="1"/>
+        <v>20.681967213114756</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="B9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1.4410000000000001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.33</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.80900000000000005</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="I9" s="6">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0.378</v>
+      </c>
+      <c r="K9" s="6">
+        <v>0.315</v>
+      </c>
+      <c r="L9">
+        <v>7.6999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>0.05</v>
       </c>
-      <c r="C9">
+      <c r="B10" s="6">
+        <v>1.645</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1.484</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1.347</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.95</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0.372</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.317</v>
+      </c>
+      <c r="L10">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1.6240000000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1.448</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.3149999999999999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="K11" s="6">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="L11">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B12" s="6">
+        <v>1.276</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1.4990000000000001</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1.5429999999999999</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0.89</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0.84</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I12" s="6">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0.373</v>
+      </c>
+      <c r="K12" s="6">
+        <v>0.31</v>
+      </c>
+      <c r="L12">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="B13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="C13">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="E13">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="G13">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="H13">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="I13">
         <v>5.2999999999999999E-2</v>
       </c>
-      <c r="D9">
+      <c r="J13">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="L13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="B14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="C14">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="D14">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="F14">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="G14">
+        <v>5.5E-2</v>
+      </c>
+      <c r="H14">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="I14">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="J14">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K14">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="L14">
+        <v>0.06</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="B8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="C8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G8">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="F9">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="G9">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="H9">
-        <v>4.9000000000000002E-2</v>
+      <c r="H8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I8">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="J8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="K8">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L8">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="N8">
+        <v>1.5149999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0.32700000000000001</v>
       </c>
       <c r="I9">
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="J9">
-        <v>7.0999999999999994E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="K9">
-        <v>6.4000000000000001E-2</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="L9">
-        <v>7.1999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="N9">
+        <f>AVERAGE(B9:B11)</f>
+        <v>0.85266666666666657</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ref="O9:S9" si="0">AVERAGE(C9:C11)</f>
+        <v>0.68166666666666664</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>0.61633333333333329</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>0.37433333333333335</v>
+      </c>
+      <c r="T9">
+        <f>AVERAGE(H9:H11)</f>
+        <v>0.30066666666666669</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.05</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.505</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="I10">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="J10">
+        <v>4.7E-2</v>
+      </c>
+      <c r="K10">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="L10">
+        <v>5.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.68</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.496</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.377</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.308</v>
+      </c>
+      <c r="I11">
+        <v>0.05</v>
+      </c>
+      <c r="J11">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="K11">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="L11">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="N11">
+        <v>1.996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="B12">
-        <v>0.106</v>
-      </c>
-      <c r="C12">
-        <v>0.125</v>
-      </c>
-      <c r="D12">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="E12">
-        <v>0.17</v>
-      </c>
-      <c r="F12">
-        <v>0.186</v>
-      </c>
-      <c r="G12">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="H12">
-        <v>0.182</v>
+        <v>4.7E-2</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.40500000000000003</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.313</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.22600000000000001</v>
       </c>
       <c r="I12">
-        <v>0.16400000000000001</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="J12">
-        <v>0.121</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="K12">
-        <v>0.115</v>
+        <v>4.7E-2</v>
       </c>
       <c r="L12">
-        <v>0.111</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="N12">
-        <f>AVERAGE(B13:B15)</f>
-        <v>1.5609999999999999</v>
+        <f>AVERAGE(B12:B14)</f>
+        <v>0.81933333333333336</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:W12" si="2">AVERAGE(C13:C15)</f>
-        <v>1.27</v>
+        <f t="shared" ref="O12:T12" si="1">AVERAGE(C12:C14)</f>
+        <v>0.64600000000000002</v>
       </c>
       <c r="P12">
+        <f t="shared" si="1"/>
+        <v>0.54333333333333333</v>
+      </c>
+      <c r="Q12">
+        <f>AVERAGE(E12:E14)</f>
+        <v>0.50166666666666659</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>0.39533333333333331</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="1"/>
+        <v>0.30233333333333334</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>0.219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.624</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.497</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.214</v>
+      </c>
+      <c r="I13">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="J13">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="K13">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L13">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.78</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.496</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.217</v>
+      </c>
+      <c r="I14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="J14">
+        <v>0.05</v>
+      </c>
+      <c r="K14">
+        <v>4.7E-2</v>
+      </c>
+      <c r="L14">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C15">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="E15">
+        <v>4.7E-2</v>
+      </c>
+      <c r="F15">
+        <v>4.7E-2</v>
+      </c>
+      <c r="G15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="H15">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="I15">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="J15">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="K15">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="L15">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0.85266666666666657</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="G19">
+        <v>0.81933333333333336</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="C20">
+        <v>0.68166666666666664</v>
+      </c>
+      <c r="D20">
+        <f>C20/0.852667*100</f>
+        <v>79.945238488960712</v>
+      </c>
+      <c r="G20">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="H20">
+        <f>G20/0.819333*100</f>
+        <v>78.844621173564349</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="C21">
+        <v>0.61633333333333329</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D25" si="2">C21/0.852667*100</f>
+        <v>72.283005362390398</v>
+      </c>
+      <c r="G21">
+        <v>0.54333333333333333</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ref="H21:H25" si="3">G21/0.819333*100</f>
+        <v>66.314103463833789</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C22">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="2"/>
-        <v>1.1536666666666664</v>
-      </c>
-      <c r="Q12">
+        <v>68.725539982197034</v>
+      </c>
+      <c r="G22">
+        <v>0.50166666666666659</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>61.22866608163794</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.49066666666666664</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="2"/>
-        <v>1.042</v>
-      </c>
-      <c r="R12">
+        <v>57.544934501589331</v>
+      </c>
+      <c r="G23">
+        <v>0.39533333333333331</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>48.250629882274161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="C24">
+        <v>0.37433333333333335</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="2"/>
-        <v>1.1143333333333334</v>
-      </c>
-      <c r="S12">
+        <v>43.901468373155453</v>
+      </c>
+      <c r="G24">
+        <v>0.30233333333333334</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>36.899933645213039</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>0.30066666666666669</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="2"/>
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="T12">
-        <f t="shared" si="2"/>
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="2"/>
-        <v>0.58966666666666667</v>
-      </c>
-      <c r="V12">
-        <f t="shared" si="2"/>
-        <v>0.46</v>
-      </c>
-      <c r="W12">
-        <f t="shared" si="2"/>
-        <v>0.39833333333333337</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0.107</v>
-      </c>
-      <c r="B13">
-        <v>1.591</v>
-      </c>
-      <c r="C13">
-        <v>1.194</v>
-      </c>
-      <c r="D13">
-        <v>1.5189999999999999</v>
-      </c>
-      <c r="E13">
-        <v>1.0409999999999999</v>
-      </c>
-      <c r="F13">
-        <v>1.089</v>
-      </c>
-      <c r="G13">
-        <v>0.96599999999999997</v>
-      </c>
-      <c r="H13">
-        <v>0.78</v>
-      </c>
-      <c r="I13">
-        <v>0.6</v>
-      </c>
-      <c r="J13">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="K13">
-        <v>0.40400000000000003</v>
-      </c>
-      <c r="L13">
-        <v>0.1</v>
-      </c>
-      <c r="N13">
-        <v>100</v>
-      </c>
-      <c r="O13">
-        <f>O12/1.561*100</f>
-        <v>81.358103779628436</v>
-      </c>
-      <c r="P13">
-        <f t="shared" ref="P13:W13" si="3">P12/1.561*100</f>
-        <v>73.905616058082416</v>
-      </c>
-      <c r="Q13">
+        <v>35.261909592685861</v>
+      </c>
+      <c r="G25">
+        <v>0.219</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="3"/>
-        <v>66.752081998718765</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="3"/>
-        <v>71.385863762545384</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="3"/>
-        <v>59.192825112107627</v>
-      </c>
-      <c r="T13">
-        <f t="shared" si="3"/>
-        <v>48.814862267777073</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="3"/>
-        <v>37.774930600042708</v>
-      </c>
-      <c r="V13">
-        <f t="shared" si="3"/>
-        <v>29.468289557975659</v>
-      </c>
-      <c r="W13">
-        <f t="shared" si="3"/>
-        <v>25.517830450565882</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0.122</v>
-      </c>
-      <c r="B14">
-        <v>1.4910000000000001</v>
-      </c>
-      <c r="C14">
-        <v>1.298</v>
-      </c>
-      <c r="D14">
-        <v>1.0569999999999999</v>
-      </c>
-      <c r="E14">
-        <v>1.0469999999999999</v>
-      </c>
-      <c r="F14">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G14">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="H14">
-        <v>0.752</v>
-      </c>
-      <c r="I14">
-        <v>0.59199999999999997</v>
-      </c>
-      <c r="J14">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="K14">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="L14">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="N14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0.155</v>
-      </c>
-      <c r="B15">
-        <v>1.601</v>
-      </c>
-      <c r="C15">
-        <v>1.3180000000000001</v>
-      </c>
-      <c r="D15">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="E15">
-        <v>1.038</v>
-      </c>
-      <c r="F15">
-        <v>1.1339999999999999</v>
-      </c>
-      <c r="G15">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="H15">
-        <v>0.754</v>
-      </c>
-      <c r="I15">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="J15">
-        <v>0.46300000000000002</v>
-      </c>
-      <c r="K15">
-        <v>0.39300000000000002</v>
-      </c>
-      <c r="L15">
-        <v>0.14899999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="B16">
-        <v>0.151</v>
-      </c>
-      <c r="C16">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="D16">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="E16">
-        <v>0.19</v>
-      </c>
-      <c r="F16">
-        <v>0.186</v>
-      </c>
-      <c r="G16">
-        <v>0.16</v>
-      </c>
-      <c r="H16">
-        <v>0.185</v>
-      </c>
-      <c r="I16">
-        <v>0.217</v>
-      </c>
-      <c r="J16">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="K16">
-        <v>0.245</v>
-      </c>
-      <c r="L16">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="B17">
-        <v>0.153</v>
-      </c>
-      <c r="C17">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="D17">
-        <v>0.23799999999999999</v>
-      </c>
-      <c r="E17">
-        <v>0.183</v>
-      </c>
-      <c r="F17">
-        <v>0.19</v>
-      </c>
-      <c r="G17">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="H17">
-        <v>0.20699999999999999</v>
-      </c>
-      <c r="I17">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="J17">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="K17">
-        <v>0.17899999999999999</v>
-      </c>
-      <c r="L17">
-        <v>0.16200000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>0.124</v>
-      </c>
-      <c r="B18">
-        <v>0.157</v>
-      </c>
-      <c r="C18">
-        <v>0.153</v>
-      </c>
-      <c r="D18">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="E18">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="F18">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="G18">
-        <v>0.128</v>
-      </c>
-      <c r="H18">
-        <v>0.161</v>
-      </c>
-      <c r="I18">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="J18">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="K18">
-        <v>0.155</v>
-      </c>
-      <c r="L18">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>0.112</v>
-      </c>
-      <c r="B19">
-        <v>0.124</v>
-      </c>
-      <c r="C19">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="D19">
-        <v>0.15</v>
-      </c>
-      <c r="E19">
-        <v>0.151</v>
-      </c>
-      <c r="F19">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="G19">
-        <v>0.155</v>
-      </c>
-      <c r="H19">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="I19">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="J19">
-        <v>0.155</v>
-      </c>
-      <c r="K19">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="L19">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="B22">
-        <v>0.1</v>
-      </c>
-      <c r="C22">
-        <v>0.111</v>
-      </c>
-      <c r="D22">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="E22">
-        <v>0.1</v>
-      </c>
-      <c r="F22">
-        <v>0.104</v>
-      </c>
-      <c r="G22">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="H22">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="I22">
-        <v>9.4E-2</v>
-      </c>
-      <c r="J22">
-        <v>0.107</v>
-      </c>
-      <c r="K22">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="L22">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="N22">
-        <f>AVERAGE(B23:B25)</f>
-        <v>1.8873333333333333</v>
-      </c>
-      <c r="O22">
-        <f t="shared" ref="O22:W22" si="4">AVERAGE(C23:C25)</f>
-        <v>1.6706666666666667</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="4"/>
-        <v>1.5486666666666666</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="4"/>
-        <v>1.0773333333333333</v>
-      </c>
-      <c r="R22">
-        <f t="shared" si="4"/>
-        <v>0.95866666666666678</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="4"/>
-        <v>0.73133333333333328</v>
-      </c>
-      <c r="T22">
-        <f t="shared" si="4"/>
-        <v>0.60133333333333339</v>
-      </c>
-      <c r="U22">
-        <f t="shared" si="4"/>
-        <v>0.49933333333333341</v>
-      </c>
-      <c r="V22">
-        <f t="shared" si="4"/>
-        <v>0.37833333333333335</v>
-      </c>
-      <c r="W22">
-        <f t="shared" si="4"/>
-        <v>0.33300000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>9.4E-2</v>
-      </c>
-      <c r="B23">
-        <v>1.9930000000000001</v>
-      </c>
-      <c r="C23">
-        <v>1.667</v>
-      </c>
-      <c r="D23">
-        <v>1.51</v>
-      </c>
-      <c r="E23">
-        <v>1.0269999999999999</v>
-      </c>
-      <c r="F23">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="G23">
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="H23">
-        <v>0.66300000000000003</v>
-      </c>
-      <c r="I23">
-        <v>0.46800000000000003</v>
-      </c>
-      <c r="J23">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="K23">
-        <v>0.32500000000000001</v>
-      </c>
-      <c r="L23">
-        <v>0.193</v>
-      </c>
-      <c r="N23">
-        <v>100</v>
-      </c>
-      <c r="O23">
-        <f>O22/1.887333*100</f>
-        <v>88.519973246198035</v>
-      </c>
-      <c r="P23">
-        <f t="shared" ref="P23:W23" si="5">P22/1.887333*100</f>
-        <v>82.055825159983257</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="5"/>
-        <v>57.082313154770958</v>
-      </c>
-      <c r="R23">
-        <f t="shared" si="5"/>
-        <v>50.794781136485547</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="5"/>
-        <v>38.749565303702809</v>
-      </c>
-      <c r="T23">
-        <f t="shared" si="5"/>
-        <v>31.861538654457554</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="5"/>
-        <v>26.457086975818971</v>
-      </c>
-      <c r="V23">
-        <f t="shared" si="5"/>
-        <v>20.045923709982997</v>
-      </c>
-      <c r="W23">
-        <f t="shared" si="5"/>
-        <v>17.643945186143622</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>0.127</v>
-      </c>
-      <c r="B24">
-        <v>1.804</v>
-      </c>
-      <c r="C24">
-        <v>1.675</v>
-      </c>
-      <c r="D24">
-        <v>1.58</v>
-      </c>
-      <c r="E24">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="F24">
-        <v>0.93600000000000005</v>
-      </c>
-      <c r="G24">
-        <v>0.76600000000000001</v>
-      </c>
-      <c r="H24">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="I24">
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="J24">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="K24">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="L24">
-        <v>0.112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>0.107</v>
-      </c>
-      <c r="B25">
-        <v>1.865</v>
-      </c>
-      <c r="C25">
-        <v>1.67</v>
-      </c>
-      <c r="D25">
-        <v>1.556</v>
-      </c>
-      <c r="E25">
-        <v>1.0649999999999999</v>
-      </c>
-      <c r="F25">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="G25">
-        <v>0.73599999999999999</v>
-      </c>
-      <c r="H25">
-        <v>0.61199999999999999</v>
-      </c>
-      <c r="I25">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="J25">
-        <v>0.37</v>
-      </c>
-      <c r="K25">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="L25">
-        <v>9.7000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0.08</v>
-      </c>
-      <c r="B26">
-        <v>0.17399999999999999</v>
-      </c>
-      <c r="C26">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="D26">
-        <v>0.122</v>
-      </c>
-      <c r="E26">
-        <v>0.192</v>
-      </c>
-      <c r="F26">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="G26">
-        <v>0.114</v>
-      </c>
-      <c r="H26">
-        <v>0.123</v>
-      </c>
-      <c r="I26">
-        <v>0.121</v>
-      </c>
-      <c r="J26">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="K26">
-        <v>0.159</v>
-      </c>
-      <c r="L26">
-        <v>0.105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>0.105</v>
-      </c>
-      <c r="B27">
-        <v>0.108</v>
-      </c>
-      <c r="C27">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="D27">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="E27">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="F27">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="G27">
-        <v>0.159</v>
-      </c>
-      <c r="H27">
-        <v>0.158</v>
-      </c>
-      <c r="I27">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="J27">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="K27">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="L27">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>0.108</v>
-      </c>
-      <c r="B28">
-        <v>0.123</v>
-      </c>
-      <c r="C28">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="D28">
-        <v>0.159</v>
-      </c>
-      <c r="E28">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="F28">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="G28">
-        <v>0.13</v>
-      </c>
-      <c r="H28">
-        <v>0.124</v>
-      </c>
-      <c r="I28">
-        <v>0.13</v>
-      </c>
-      <c r="J28">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="K28">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="L28">
-        <v>0.111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>0.112</v>
-      </c>
-      <c r="B29">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="C29">
-        <v>0.157</v>
-      </c>
-      <c r="D29">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="E29">
-        <v>0.113</v>
-      </c>
-      <c r="F29">
-        <v>0.14599999999999999</v>
-      </c>
-      <c r="G29">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="H29">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="I29">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="J29">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="K29">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="L29">
-        <v>0.112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="B32">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="C32">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="D32">
-        <v>5.5E-2</v>
-      </c>
-      <c r="E32">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="F32">
-        <v>6.3E-2</v>
-      </c>
-      <c r="G32">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="H32">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="I32">
-        <v>4.7E-2</v>
-      </c>
-      <c r="J32">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="K32">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="L32">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="N32">
-        <f>AVERAGE(B33:B37)</f>
-        <v>1.5249999999999999</v>
-      </c>
-      <c r="O32">
-        <f t="shared" ref="O32:W32" si="6">AVERAGE(C33:C37)</f>
-        <v>1.4758000000000002</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="6"/>
-        <v>1.3779999999999999</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="6"/>
-        <v>0.93599999999999994</v>
-      </c>
-      <c r="R32">
-        <f t="shared" si="6"/>
-        <v>0.82279999999999998</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="6"/>
-        <v>0.61080000000000001</v>
-      </c>
-      <c r="T32">
-        <f t="shared" si="6"/>
-        <v>0.5292</v>
-      </c>
-      <c r="U32">
-        <f t="shared" si="6"/>
-        <v>0.41259999999999997</v>
-      </c>
-      <c r="V32">
-        <f t="shared" si="6"/>
-        <v>0.36799999999999999</v>
-      </c>
-      <c r="W32">
-        <f t="shared" si="6"/>
-        <v>0.31540000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="B33">
-        <v>1.456</v>
-      </c>
-      <c r="C33">
-        <v>1.5069999999999999</v>
-      </c>
-      <c r="D33">
-        <v>1.355</v>
-      </c>
-      <c r="E33">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="F33">
-        <v>0.81599999999999995</v>
-      </c>
-      <c r="G33">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="H33">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="I33">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="J33">
-        <v>0.35899999999999999</v>
-      </c>
-      <c r="K33">
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="L33">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="N33">
-        <v>100</v>
-      </c>
-      <c r="O33">
-        <f>O32/1.525*100</f>
-        <v>96.773770491803305</v>
-      </c>
-      <c r="P33">
-        <f t="shared" ref="P33:W33" si="7">P32/1.525*100</f>
-        <v>90.360655737704917</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="7"/>
-        <v>61.377049180327873</v>
-      </c>
-      <c r="R33">
-        <f t="shared" si="7"/>
-        <v>53.954098360655742</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="7"/>
-        <v>40.052459016393442</v>
-      </c>
-      <c r="T33">
-        <f t="shared" si="7"/>
-        <v>34.701639344262297</v>
-      </c>
-      <c r="U33">
-        <f t="shared" si="7"/>
-        <v>27.05573770491803</v>
-      </c>
-      <c r="V33">
-        <f t="shared" si="7"/>
-        <v>24.131147540983608</v>
-      </c>
-      <c r="W33">
-        <f t="shared" si="7"/>
-        <v>20.681967213114756</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="B34">
-        <v>1.6240000000000001</v>
-      </c>
-      <c r="C34">
-        <v>1.4410000000000001</v>
-      </c>
-      <c r="D34">
-        <v>1.33</v>
-      </c>
-      <c r="E34">
-        <v>0.95799999999999996</v>
-      </c>
-      <c r="F34">
-        <v>0.80900000000000005</v>
-      </c>
-      <c r="G34">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="H34">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="I34">
-        <v>0.42799999999999999</v>
-      </c>
-      <c r="J34">
-        <v>0.378</v>
-      </c>
-      <c r="K34">
-        <v>0.315</v>
-      </c>
-      <c r="L34">
-        <v>7.6999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>0.05</v>
-      </c>
-      <c r="B35">
-        <v>1.645</v>
-      </c>
-      <c r="C35">
-        <v>1.484</v>
-      </c>
-      <c r="D35">
-        <v>1.347</v>
-      </c>
-      <c r="E35">
-        <v>0.95</v>
-      </c>
-      <c r="F35">
-        <v>0.82699999999999996</v>
-      </c>
-      <c r="G35">
-        <v>0.63600000000000001</v>
-      </c>
-      <c r="H35">
-        <v>0.50800000000000001</v>
-      </c>
-      <c r="I35">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="J35">
-        <v>0.372</v>
-      </c>
-      <c r="K35">
-        <v>0.317</v>
-      </c>
-      <c r="L35">
-        <v>6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="B36">
-        <v>1.6240000000000001</v>
-      </c>
-      <c r="C36">
-        <v>1.448</v>
-      </c>
-      <c r="D36">
-        <v>1.3149999999999999</v>
-      </c>
-      <c r="E36">
-        <v>0.97599999999999998</v>
-      </c>
-      <c r="F36">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="G36">
-        <v>0.58599999999999997</v>
-      </c>
-      <c r="H36">
-        <v>0.53500000000000003</v>
-      </c>
-      <c r="I36">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="J36">
-        <v>0.35799999999999998</v>
-      </c>
-      <c r="K36">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="L36">
-        <v>6.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="B37">
-        <v>1.276</v>
-      </c>
-      <c r="C37">
-        <v>1.4990000000000001</v>
-      </c>
-      <c r="D37">
-        <v>1.5429999999999999</v>
-      </c>
-      <c r="E37">
-        <v>0.89</v>
-      </c>
-      <c r="F37">
-        <v>0.84</v>
-      </c>
-      <c r="G37">
-        <v>0.57699999999999996</v>
-      </c>
-      <c r="H37">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="I37">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="J37">
-        <v>0.373</v>
-      </c>
-      <c r="K37">
-        <v>0.31</v>
-      </c>
-      <c r="L37">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="B38">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="C38">
-        <v>5.5E-2</v>
-      </c>
-      <c r="D38">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="E38">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="F38">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="G38">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="H38">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="I38">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="J38">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="K38">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="L38">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="B39">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="C39">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="D39">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E39">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="F39">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="G39">
-        <v>5.5E-2</v>
-      </c>
-      <c r="H39">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="I39">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="J39">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="K39">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="L39">
-        <v>0.06</v>
+        <v>26.729058880821349</v>
       </c>
     </row>
   </sheetData>
@@ -4134,7 +4889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -6070,7 +6825,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C27"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>